<commit_message>
Updated spreadsheets 1-4  "/" was causing an nesting issue in firebase.
playing around with the snapshot in ytdData trying to figure out how to calculate the total wins for each user
</commit_message>
<xml_diff>
--- a/src/utils/spreadsheets/week 1.xlsx
+++ b/src/utils/spreadsheets/week 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordy\pick-em-1\src\utils\spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordyfigueroa/Desktop/pick-em/src/utils/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C523041-2077-448B-A75F-8F5EE9810D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C016CA01-3FC9-3A47-BB0D-78C6B883E8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{91822C31-101A-4E46-AC5B-8A5B4D3049B0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19260" xr2:uid="{91822C31-101A-4E46-AC5B-8A5B4D3049B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Table001 (Page 1)" sheetId="2" r:id="rId1"/>
@@ -237,7 +237,7 @@
     <t>DONTE</t>
   </si>
   <si>
-    <t>ANN/TERRI</t>
+    <t>ANN TERRI</t>
   </si>
 </sst>
 </file>
@@ -273,9 +273,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,20 +378,20 @@
     <tableColumn id="1" xr3:uid="{C3158AA3-1F1C-4107-BB38-A22912875472}" uniqueName="1" name="Away" queryTableFieldId="1" dataDxfId="16"/>
     <tableColumn id="2" xr3:uid="{1356EE8D-3DD3-4B80-91ED-32503AC75872}" uniqueName="2" name="CHIEFS" queryTableFieldId="2" dataDxfId="15"/>
     <tableColumn id="3" xr3:uid="{AB038BD1-E5C1-49EF-84FC-3A90DB77CCBF}" uniqueName="3" name="FALCONS" queryTableFieldId="3" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{4949B450-38D3-48E0-BCA0-4F9120EE4016}" uniqueName="5" name="BROWNS" queryTableFieldId="5" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{44AEEFAA-E770-4417-A000-36C54305BA61}" uniqueName="6" name="COLTS" queryTableFieldId="6" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{20D32888-5234-45F6-A444-85ACC8C3FE9D}" uniqueName="7" name="VIKINGS" queryTableFieldId="7" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{F9D24EE2-500E-434C-BAE6-58DCD9A0A013}" uniqueName="8" name="SAINTS" queryTableFieldId="8" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{64C3C588-7173-4B31-9823-B47DBB943588}" uniqueName="9" name="STEELERS" queryTableFieldId="9" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{E09BC055-D182-40DA-BFE1-ABC661A1069E}" uniqueName="10" name="COMMANDERS" queryTableFieldId="10" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{131B532B-DECD-414A-AE46-9C2EE0AF1AB9}" uniqueName="4" name="RAVENS" queryTableFieldId="4" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{2DE08440-A113-4664-B5E2-C7ACFF3CA1A6}" uniqueName="11" name="BEARS" queryTableFieldId="11" dataDxfId="11"/>
-    <tableColumn id="15" xr3:uid="{0146C24F-6629-43AC-8B1E-EE0B86B9DD50}" uniqueName="15" name="BRONCOS" queryTableFieldId="15" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{E6F789C8-7075-44F0-9CEE-B36E872D5599}" uniqueName="13" name="PATRIOTS" queryTableFieldId="13" dataDxfId="0"/>
-    <tableColumn id="12" xr3:uid="{482AC0FB-5421-4A5F-A479-E2A0EE84C324}" uniqueName="12" name="CHARGERS" queryTableFieldId="12" dataDxfId="10"/>
-    <tableColumn id="14" xr3:uid="{ED2253EA-DA0F-4628-AB5A-71595AE923C5}" uniqueName="14" name="SEAHAWKS" queryTableFieldId="14" dataDxfId="9"/>
-    <tableColumn id="16" xr3:uid="{8995A089-157F-41AC-BA5E-9477CCD83656}" uniqueName="16" name="GIANTS" queryTableFieldId="16" dataDxfId="8"/>
-    <tableColumn id="17" xr3:uid="{73DD9AF1-A1D6-43E3-A40C-618A3828D9BC}" uniqueName="17" name="JETS" queryTableFieldId="17" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{4949B450-38D3-48E0-BCA0-4F9120EE4016}" uniqueName="5" name="BROWNS" queryTableFieldId="5" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{44AEEFAA-E770-4417-A000-36C54305BA61}" uniqueName="6" name="COLTS" queryTableFieldId="6" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{20D32888-5234-45F6-A444-85ACC8C3FE9D}" uniqueName="7" name="VIKINGS" queryTableFieldId="7" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{F9D24EE2-500E-434C-BAE6-58DCD9A0A013}" uniqueName="8" name="SAINTS" queryTableFieldId="8" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{64C3C588-7173-4B31-9823-B47DBB943588}" uniqueName="9" name="STEELERS" queryTableFieldId="9" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{E09BC055-D182-40DA-BFE1-ABC661A1069E}" uniqueName="10" name="COMMANDERS" queryTableFieldId="10" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{131B532B-DECD-414A-AE46-9C2EE0AF1AB9}" uniqueName="4" name="RAVENS" queryTableFieldId="4" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{2DE08440-A113-4664-B5E2-C7ACFF3CA1A6}" uniqueName="11" name="BEARS" queryTableFieldId="11" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{0146C24F-6629-43AC-8B1E-EE0B86B9DD50}" uniqueName="15" name="BRONCOS" queryTableFieldId="15" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{E6F789C8-7075-44F0-9CEE-B36E872D5599}" uniqueName="13" name="PATRIOTS" queryTableFieldId="13" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{482AC0FB-5421-4A5F-A479-E2A0EE84C324}" uniqueName="12" name="CHARGERS" queryTableFieldId="12" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{ED2253EA-DA0F-4628-AB5A-71595AE923C5}" uniqueName="14" name="SEAHAWKS" queryTableFieldId="14" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{8995A089-157F-41AC-BA5E-9477CCD83656}" uniqueName="16" name="GIANTS" queryTableFieldId="16" dataDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{73DD9AF1-A1D6-43E3-A40C-618A3828D9BC}" uniqueName="17" name="JETS" queryTableFieldId="17" dataDxfId="0"/>
     <tableColumn id="18" xr3:uid="{6D5C6E45-8CAA-4720-9FDE-F240EBED2AF7}" uniqueName="18" name="Tie Breaker_x000a_Score_x000a_(Combined_x000a_Monday Night_x000a_Scores)" queryTableFieldId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -699,31 +698,31 @@
   <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:O1048576"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="53" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -779,1568 +778,1568 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="1" t="s">
+      <c r="M2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" t="s">
         <v>33</v>
       </c>
       <c r="R2">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="J3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N3" s="1" t="s">
+      <c r="M3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" t="s">
         <v>16</v>
       </c>
       <c r="R3">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K4" s="1" t="s">
+      <c r="J4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N4" s="1" t="s">
+      <c r="M4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="O4" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="P4" t="s">
         <v>32</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="Q4" t="s">
         <v>33</v>
       </c>
       <c r="R4">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="1" t="s">
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K5" s="1" t="s">
+      <c r="J5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N5" s="1" t="s">
+      <c r="M5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" t="s">
         <v>11</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" t="s">
         <v>30</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="P5" t="s">
         <v>32</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" t="s">
         <v>33</v>
       </c>
       <c r="R5">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K6" s="1" t="s">
+      <c r="J6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="L6" t="s">
         <v>31</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N6" s="1" t="s">
+      <c r="M6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" t="s">
         <v>11</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="O6" t="s">
         <v>13</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="P6" t="s">
         <v>32</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6" t="s">
         <v>33</v>
       </c>
       <c r="R6">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K7" s="1" t="s">
+      <c r="J7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" t="s">
         <v>27</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" t="s">
         <v>31</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N7" s="1" t="s">
+      <c r="M7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" t="s">
         <v>28</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O7" t="s">
         <v>13</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P7" t="s">
         <v>32</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" t="s">
         <v>33</v>
       </c>
       <c r="R7">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="1" t="s">
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K8" s="1" t="s">
+      <c r="J8" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L8" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N8" s="1" t="s">
+      <c r="M8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N8" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O8" t="s">
         <v>13</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="P8" t="s">
         <v>32</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q8" t="s">
         <v>33</v>
       </c>
       <c r="R8">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" s="1" t="s">
+      <c r="J9" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" t="s">
         <v>27</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="L9" t="s">
         <v>31</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="M9" t="s">
         <v>12</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="N9" t="s">
         <v>11</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="O9" t="s">
         <v>30</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="P9" t="s">
         <v>15</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="Q9" t="s">
         <v>33</v>
       </c>
       <c r="R9">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K10" s="1" t="s">
+      <c r="J10" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" t="s">
         <v>10</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="L10" t="s">
         <v>31</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N10" s="1" t="s">
+      <c r="M10" t="s">
+        <v>29</v>
+      </c>
+      <c r="N10" t="s">
         <v>11</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="O10" t="s">
         <v>13</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="P10" t="s">
         <v>15</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="Q10" t="s">
         <v>33</v>
       </c>
       <c r="R10">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="1" t="s">
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K11" s="1" t="s">
+      <c r="J11" t="s">
+        <v>3</v>
+      </c>
+      <c r="K11" t="s">
         <v>27</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="L11" t="s">
         <v>31</v>
       </c>
-      <c r="M11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N11" s="1" t="s">
+      <c r="M11" t="s">
+        <v>29</v>
+      </c>
+      <c r="N11" t="s">
         <v>11</v>
       </c>
-      <c r="O11" s="1" t="s">
+      <c r="O11" t="s">
         <v>30</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="P11" t="s">
         <v>15</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="Q11" t="s">
         <v>16</v>
       </c>
       <c r="R11">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" s="1" t="s">
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K12" s="1" t="s">
+      <c r="J12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K12" t="s">
         <v>10</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="L12" t="s">
         <v>14</v>
       </c>
-      <c r="M12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N12" s="1" t="s">
+      <c r="M12" t="s">
+        <v>29</v>
+      </c>
+      <c r="N12" t="s">
         <v>11</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="O12" t="s">
         <v>13</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="P12" t="s">
         <v>32</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="Q12" t="s">
         <v>33</v>
       </c>
       <c r="R12">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" s="1" t="s">
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I13" t="s">
         <v>9</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" t="s">
         <v>20</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="K13" t="s">
         <v>10</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="L13" t="s">
         <v>31</v>
       </c>
-      <c r="M13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N13" s="1" t="s">
+      <c r="M13" t="s">
+        <v>29</v>
+      </c>
+      <c r="N13" t="s">
         <v>11</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="O13" t="s">
         <v>30</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="P13" t="s">
         <v>32</v>
       </c>
-      <c r="Q13" s="1" t="s">
+      <c r="Q13" t="s">
         <v>33</v>
       </c>
       <c r="R13">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="1" t="s">
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I14" t="s">
         <v>9</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K14" s="1" t="s">
+      <c r="J14" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" t="s">
         <v>10</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="L14" t="s">
         <v>31</v>
       </c>
-      <c r="M14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N14" s="1" t="s">
+      <c r="M14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N14" t="s">
         <v>11</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="O14" t="s">
         <v>13</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="P14" t="s">
         <v>32</v>
       </c>
-      <c r="Q14" s="1" t="s">
+      <c r="Q14" t="s">
         <v>33</v>
       </c>
       <c r="R14">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" s="1" t="s">
+      <c r="F15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="I15" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K15" s="1" t="s">
+      <c r="J15" t="s">
+        <v>3</v>
+      </c>
+      <c r="K15" t="s">
         <v>10</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="L15" t="s">
         <v>14</v>
       </c>
-      <c r="M15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N15" s="1" t="s">
+      <c r="M15" t="s">
+        <v>29</v>
+      </c>
+      <c r="N15" t="s">
         <v>11</v>
       </c>
-      <c r="O15" s="1" t="s">
+      <c r="O15" t="s">
         <v>13</v>
       </c>
-      <c r="P15" s="1" t="s">
+      <c r="P15" t="s">
         <v>32</v>
       </c>
-      <c r="Q15" s="1" t="s">
+      <c r="Q15" t="s">
         <v>33</v>
       </c>
       <c r="R15">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="1" t="s">
+      <c r="F16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" t="s">
         <v>24</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K16" s="1" t="s">
+      <c r="J16" t="s">
+        <v>3</v>
+      </c>
+      <c r="K16" t="s">
         <v>10</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="L16" t="s">
         <v>31</v>
       </c>
-      <c r="M16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N16" s="1" t="s">
+      <c r="M16" t="s">
+        <v>29</v>
+      </c>
+      <c r="N16" t="s">
         <v>28</v>
       </c>
-      <c r="O16" s="1" t="s">
+      <c r="O16" t="s">
         <v>30</v>
       </c>
-      <c r="P16" s="1" t="s">
+      <c r="P16" t="s">
         <v>32</v>
       </c>
-      <c r="Q16" s="1" t="s">
+      <c r="Q16" t="s">
         <v>16</v>
       </c>
       <c r="R16">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" s="1" t="s">
+      <c r="F17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" t="s">
         <v>7</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" t="s">
         <v>8</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I17" t="s">
         <v>26</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="J17" t="s">
         <v>20</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="K17" t="s">
         <v>10</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="L17" t="s">
         <v>31</v>
       </c>
-      <c r="M17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N17" s="1" t="s">
+      <c r="M17" t="s">
+        <v>29</v>
+      </c>
+      <c r="N17" t="s">
         <v>28</v>
       </c>
-      <c r="O17" s="1" t="s">
+      <c r="O17" t="s">
         <v>30</v>
       </c>
-      <c r="P17" s="1" t="s">
+      <c r="P17" t="s">
         <v>15</v>
       </c>
-      <c r="Q17" s="1" t="s">
+      <c r="Q17" t="s">
         <v>33</v>
       </c>
       <c r="R17">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G18" s="1" t="s">
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" t="s">
         <v>24</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" t="s">
         <v>25</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I18" t="s">
         <v>9</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K18" s="1" t="s">
+      <c r="J18" t="s">
+        <v>3</v>
+      </c>
+      <c r="K18" t="s">
         <v>10</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="L18" t="s">
         <v>31</v>
       </c>
-      <c r="M18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N18" s="1" t="s">
+      <c r="M18" t="s">
+        <v>29</v>
+      </c>
+      <c r="N18" t="s">
         <v>11</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="O18" t="s">
         <v>30</v>
       </c>
-      <c r="P18" s="1" t="s">
+      <c r="P18" t="s">
         <v>32</v>
       </c>
-      <c r="Q18" s="1" t="s">
+      <c r="Q18" t="s">
         <v>33</v>
       </c>
       <c r="R18">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G19" s="1" t="s">
+      <c r="F19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" t="s">
         <v>7</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I19" t="s">
         <v>9</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K19" s="1" t="s">
+      <c r="J19" t="s">
+        <v>3</v>
+      </c>
+      <c r="K19" t="s">
         <v>27</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="L19" t="s">
         <v>14</v>
       </c>
-      <c r="M19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N19" s="1" t="s">
+      <c r="M19" t="s">
+        <v>29</v>
+      </c>
+      <c r="N19" t="s">
         <v>11</v>
       </c>
-      <c r="O19" s="1" t="s">
+      <c r="O19" t="s">
         <v>13</v>
       </c>
-      <c r="P19" s="1" t="s">
+      <c r="P19" t="s">
         <v>32</v>
       </c>
-      <c r="Q19" s="1" t="s">
+      <c r="Q19" t="s">
         <v>16</v>
       </c>
       <c r="R19">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G20" s="1" t="s">
+      <c r="F20" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" t="s">
         <v>7</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="I20" t="s">
         <v>9</v>
       </c>
-      <c r="J20" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K20" s="1" t="s">
+      <c r="J20" t="s">
+        <v>3</v>
+      </c>
+      <c r="K20" t="s">
         <v>27</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="L20" t="s">
         <v>14</v>
       </c>
-      <c r="M20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N20" s="1" t="s">
+      <c r="M20" t="s">
+        <v>29</v>
+      </c>
+      <c r="N20" t="s">
         <v>11</v>
       </c>
-      <c r="O20" s="1" t="s">
+      <c r="O20" t="s">
         <v>13</v>
       </c>
-      <c r="P20" s="1" t="s">
+      <c r="P20" t="s">
         <v>32</v>
       </c>
-      <c r="Q20" s="1" t="s">
+      <c r="Q20" t="s">
         <v>33</v>
       </c>
       <c r="R20">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G21" s="1" t="s">
+      <c r="F21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" t="s">
         <v>24</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H21" t="s">
         <v>8</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="I21" t="s">
         <v>26</v>
       </c>
-      <c r="J21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K21" s="1" t="s">
+      <c r="J21" t="s">
+        <v>3</v>
+      </c>
+      <c r="K21" t="s">
         <v>27</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="L21" t="s">
         <v>31</v>
       </c>
-      <c r="M21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N21" s="1" t="s">
+      <c r="M21" t="s">
+        <v>29</v>
+      </c>
+      <c r="N21" t="s">
         <v>28</v>
       </c>
-      <c r="O21" s="1" t="s">
+      <c r="O21" t="s">
         <v>13</v>
       </c>
-      <c r="P21" s="1" t="s">
+      <c r="P21" t="s">
         <v>32</v>
       </c>
-      <c r="Q21" s="1" t="s">
+      <c r="Q21" t="s">
         <v>33</v>
       </c>
       <c r="R21">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G22" s="1" t="s">
+      <c r="F22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" t="s">
         <v>24</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H22" t="s">
         <v>25</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I22" t="s">
         <v>26</v>
       </c>
-      <c r="J22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K22" s="1" t="s">
+      <c r="J22" t="s">
+        <v>3</v>
+      </c>
+      <c r="K22" t="s">
         <v>27</v>
       </c>
-      <c r="L22" s="1" t="s">
+      <c r="L22" t="s">
         <v>31</v>
       </c>
-      <c r="M22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N22" s="1" t="s">
+      <c r="M22" t="s">
+        <v>29</v>
+      </c>
+      <c r="N22" t="s">
         <v>28</v>
       </c>
-      <c r="O22" s="1" t="s">
+      <c r="O22" t="s">
         <v>13</v>
       </c>
-      <c r="P22" s="1" t="s">
+      <c r="P22" t="s">
         <v>32</v>
       </c>
-      <c r="Q22" s="1" t="s">
+      <c r="Q22" t="s">
         <v>33</v>
       </c>
       <c r="R22">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" s="1" t="s">
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" t="s">
         <v>4</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G23" s="1" t="s">
+      <c r="F23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" t="s">
         <v>7</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="H23" t="s">
         <v>25</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="I23" t="s">
         <v>26</v>
       </c>
-      <c r="J23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K23" s="1" t="s">
+      <c r="J23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K23" t="s">
         <v>27</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="L23" t="s">
         <v>14</v>
       </c>
-      <c r="M23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N23" s="1" t="s">
+      <c r="M23" t="s">
+        <v>29</v>
+      </c>
+      <c r="N23" t="s">
         <v>11</v>
       </c>
-      <c r="O23" s="1" t="s">
+      <c r="O23" t="s">
         <v>13</v>
       </c>
-      <c r="P23" s="1" t="s">
+      <c r="P23" t="s">
         <v>15</v>
       </c>
-      <c r="Q23" s="1" t="s">
+      <c r="Q23" t="s">
         <v>33</v>
       </c>
       <c r="R23">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G24" s="1" t="s">
+      <c r="F24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H24" t="s">
         <v>25</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="I24" t="s">
         <v>9</v>
       </c>
-      <c r="J24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K24" s="1" t="s">
+      <c r="J24" t="s">
+        <v>3</v>
+      </c>
+      <c r="K24" t="s">
         <v>27</v>
       </c>
-      <c r="L24" s="1" t="s">
+      <c r="L24" t="s">
         <v>31</v>
       </c>
-      <c r="M24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N24" s="1" t="s">
+      <c r="M24" t="s">
+        <v>29</v>
+      </c>
+      <c r="N24" t="s">
         <v>11</v>
       </c>
-      <c r="O24" s="1" t="s">
+      <c r="O24" t="s">
         <v>13</v>
       </c>
-      <c r="P24" s="1" t="s">
+      <c r="P24" t="s">
         <v>32</v>
       </c>
-      <c r="Q24" s="1" t="s">
+      <c r="Q24" t="s">
         <v>33</v>
       </c>
       <c r="R24">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" t="s">
         <v>22</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G25" s="1" t="s">
+      <c r="F25" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" t="s">
         <v>7</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H25" t="s">
         <v>25</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="I25" t="s">
         <v>9</v>
       </c>
-      <c r="J25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K25" s="1" t="s">
+      <c r="J25" t="s">
+        <v>3</v>
+      </c>
+      <c r="K25" t="s">
         <v>10</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="L25" t="s">
         <v>14</v>
       </c>
-      <c r="M25" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N25" s="1" t="s">
+      <c r="M25" t="s">
+        <v>29</v>
+      </c>
+      <c r="N25" t="s">
         <v>11</v>
       </c>
-      <c r="O25" s="1" t="s">
+      <c r="O25" t="s">
         <v>13</v>
       </c>
-      <c r="P25" s="1" t="s">
+      <c r="P25" t="s">
         <v>15</v>
       </c>
-      <c r="Q25" s="1" t="s">
+      <c r="Q25" t="s">
         <v>33</v>
       </c>
       <c r="R25">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" t="s">
         <v>4</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
         <v>22</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" t="s">
         <v>23</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G26" t="s">
         <v>24</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="H26" t="s">
         <v>8</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="I26" t="s">
         <v>9</v>
       </c>
-      <c r="J26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K26" s="1" t="s">
+      <c r="J26" t="s">
+        <v>3</v>
+      </c>
+      <c r="K26" t="s">
         <v>10</v>
       </c>
-      <c r="L26" s="1" t="s">
+      <c r="L26" t="s">
         <v>14</v>
       </c>
-      <c r="M26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N26" s="1" t="s">
+      <c r="M26" t="s">
+        <v>29</v>
+      </c>
+      <c r="N26" t="s">
         <v>11</v>
       </c>
-      <c r="O26" s="1" t="s">
+      <c r="O26" t="s">
         <v>13</v>
       </c>
-      <c r="P26" s="1" t="s">
+      <c r="P26" t="s">
         <v>15</v>
       </c>
-      <c r="Q26" s="1" t="s">
+      <c r="Q26" t="s">
         <v>33</v>
       </c>
       <c r="R26">
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>22</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G27" s="1" t="s">
+      <c r="F27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" t="s">
         <v>7</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="H27" t="s">
         <v>25</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="I27" t="s">
         <v>9</v>
       </c>
-      <c r="J27" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K27" s="1" t="s">
+      <c r="J27" t="s">
+        <v>3</v>
+      </c>
+      <c r="K27" t="s">
         <v>27</v>
       </c>
-      <c r="L27" s="1" t="s">
+      <c r="L27" t="s">
         <v>31</v>
       </c>
-      <c r="M27" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N27" s="1" t="s">
+      <c r="M27" t="s">
+        <v>29</v>
+      </c>
+      <c r="N27" t="s">
         <v>28</v>
       </c>
-      <c r="O27" s="1" t="s">
+      <c r="O27" t="s">
         <v>13</v>
       </c>
-      <c r="P27" s="1" t="s">
+      <c r="P27" t="s">
         <v>15</v>
       </c>
-      <c r="Q27" s="1" t="s">
+      <c r="Q27" t="s">
         <v>16</v>
       </c>
       <c r="R27">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
         <v>2</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
         <v>22</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G28" s="1" t="s">
+      <c r="F28" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28" t="s">
         <v>7</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="H28" t="s">
         <v>8</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="I28" t="s">
         <v>9</v>
       </c>
-      <c r="J28" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K28" s="1" t="s">
+      <c r="J28" t="s">
+        <v>3</v>
+      </c>
+      <c r="K28" t="s">
         <v>10</v>
       </c>
-      <c r="L28" s="1" t="s">
+      <c r="L28" t="s">
         <v>31</v>
       </c>
-      <c r="M28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N28" s="1" t="s">
+      <c r="M28" t="s">
+        <v>29</v>
+      </c>
+      <c r="N28" t="s">
         <v>11</v>
       </c>
-      <c r="O28" s="1" t="s">
+      <c r="O28" t="s">
         <v>13</v>
       </c>
-      <c r="P28" s="1" t="s">
+      <c r="P28" t="s">
         <v>15</v>
       </c>
-      <c r="Q28" s="1" t="s">
+      <c r="Q28" t="s">
         <v>16</v>
       </c>
       <c r="R28">
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" t="s">
         <v>4</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" t="s">
         <v>22</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" t="s">
         <v>23</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G29" t="s">
         <v>24</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="H29" t="s">
         <v>8</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="I29" t="s">
         <v>26</v>
       </c>
-      <c r="J29" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K29" s="1" t="s">
+      <c r="J29" t="s">
+        <v>3</v>
+      </c>
+      <c r="K29" t="s">
         <v>27</v>
       </c>
-      <c r="L29" s="1" t="s">
+      <c r="L29" t="s">
         <v>31</v>
       </c>
-      <c r="M29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N29" s="1" t="s">
+      <c r="M29" t="s">
+        <v>29</v>
+      </c>
+      <c r="N29" t="s">
         <v>11</v>
       </c>
-      <c r="O29" s="1" t="s">
+      <c r="O29" t="s">
         <v>30</v>
       </c>
-      <c r="P29" s="1" t="s">
+      <c r="P29" t="s">
         <v>15</v>
       </c>
-      <c r="Q29" s="1" t="s">
+      <c r="Q29" t="s">
         <v>33</v>
       </c>
       <c r="R29">
@@ -2361,7 +2360,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>